<commit_message>
Tests for project group imports
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/project_groups/project_group_import.xlsx
+++ b/spec/fixtures/files/project_groups/project_group_import.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot/Sites/hmis-warehouse/spec/fixtures/files/project_groups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835831BB-3F04-464D-95B4-A19C4D221B36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5286C59E-7ED3-9D45-8BAA-BA87F00A325D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42580" yWindow="2700" windowWidth="19960" windowHeight="14640" xr2:uid="{00600863-D3FA-8C49-8721-F89CD36AEB7C}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,7 +462,7 @@
         <v>958</v>
       </c>
       <c r="D2">
-        <v>82</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -476,7 +476,7 @@
         <v>882</v>
       </c>
       <c r="D3">
-        <v>82</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -490,7 +490,7 @@
         <v>240</v>
       </c>
       <c r="D4">
-        <v>82</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -504,7 +504,7 @@
         <v>2222</v>
       </c>
       <c r="D5">
-        <v>82</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -518,7 +518,7 @@
         <v>958</v>
       </c>
       <c r="D6">
-        <v>82</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -532,7 +532,7 @@
         <v>882</v>
       </c>
       <c r="D7">
-        <v>82</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -546,7 +546,7 @@
         <v>2222</v>
       </c>
       <c r="D9">
-        <v>82</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -560,7 +560,7 @@
         <v>240</v>
       </c>
       <c r="D10">
-        <v>82</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>